<commit_message>
İlk commit: RuhHaliOnerici Streamlit projesi
</commit_message>
<xml_diff>
--- a/gecmis_log.xlsx
+++ b/gecmis_log.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,54 +440,200 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>tarih</t>
+          <t>Tarih</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>ruh_hali</t>
+          <t>Kullanıcı</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>müzik</t>
+          <t>Ruh Hali</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>aktivite</t>
+          <t>Müzik</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>mesaj</t>
+          <t>Aktivite</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Mesaj</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-22 19:06:13</t>
+          <t>2025-11-22 19:59:10</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>kızgın</t>
+          <t>merve</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Let It Be - Beatles</t>
+          <t>Mutlu</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Derin nefes egzersizi</t>
+          <t>Happy - Pharrell</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Sakin ol, nefes al ve devam et 😤</t>
+          <t>Dans etmek</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-11-22 19:59:19</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ibrahim</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Mutlu</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Happy - Pharrell</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Dans etmek</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-11-22 19:59:28</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>hanife</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Mutlu</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Happy - Pharrell</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Dans etmek</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-11-22 20:02:00</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Yorgun</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Easy On Me - Adele</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Kısa uyku</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45983.83710914352</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ahmet</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Motivasyonlu</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Stronger - Kanye</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Hedef belirle</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Devam et, harika işler başarabilirsin 💪</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45983.83731133936</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ahmet</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Motivasyonlu</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Eye of the Tiger - Survivor</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Hedef belirle</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Devam et, harika işler başarabilirsin 💪</t>
         </is>
       </c>
     </row>

</xml_diff>